<commit_message>
Added header and footer checks
</commit_message>
<xml_diff>
--- a/Login.xlsx
+++ b/Login.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration" sheetId="2" r:id="rId1"/>
@@ -12,13 +12,15 @@
     <sheet name="LoginSuccessful" sheetId="4" r:id="rId3"/>
     <sheet name="MissingUserID" sheetId="3" r:id="rId4"/>
     <sheet name="IncorrectUserID" sheetId="5" r:id="rId5"/>
+    <sheet name="LoginHeaderFooter" sheetId="6" r:id="rId6"/>
+    <sheet name="ForgotPasswordHeaderFooter" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Site URL</t>
   </si>
@@ -63,6 +65,31 @@
   </si>
   <si>
     <t>Incorrect User ID Text</t>
+  </si>
+  <si>
+    <t>At vidit veritus duo, erat putent eu qui. Vim an numquam accumsan deserunt. Soluta delectus vim cu, ad nam agam epicuri democritum, ei torquatos scriptorem eum. Putent iracundia intellegat has an, mollis accusata scripserit pri ut. Exerci voluptua disputa</t>
+  </si>
+  <si>
+    <t>Header Text</t>
+  </si>
+  <si>
+    <t>Footer Text</t>
+  </si>
+  <si>
+    <t>© 2014 - Reviewer Connect
+Reviewer Connect Description</t>
+  </si>
+  <si>
+    <t>Please enter your e-mail address in the space provided and click Send.</t>
+  </si>
+  <si>
+    <t>Header Text 1</t>
+  </si>
+  <si>
+    <t>You will receive an e-mail with information for accessing your account.</t>
+  </si>
+  <si>
+    <t>Header Text 2</t>
   </si>
 </sst>
 </file>
@@ -98,9 +125,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,7 +434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -564,4 +594,70 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Additions to Forgot Password
</commit_message>
<xml_diff>
--- a/Login.xlsx
+++ b/Login.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration" sheetId="2" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="IncorrectUserID" sheetId="5" r:id="rId5"/>
     <sheet name="LoginHeaderFooter" sheetId="6" r:id="rId6"/>
     <sheet name="ForgotPasswordHeaderFooter" sheetId="7" r:id="rId7"/>
+    <sheet name="ForgotPasswordEmail" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>Site URL</t>
   </si>
@@ -90,6 +91,36 @@
   </si>
   <si>
     <t>Header Text 2</t>
+  </si>
+  <si>
+    <t>E-Mail Address</t>
+  </si>
+  <si>
+    <t>me.automaton@gmail.com</t>
+  </si>
+  <si>
+    <t>Default E-Mail Address Text</t>
+  </si>
+  <si>
+    <t>Enter e-mail address</t>
+  </si>
+  <si>
+    <t>Missing E-Mail Address Text</t>
+  </si>
+  <si>
+    <t>E-mail Address is Required.</t>
+  </si>
+  <si>
+    <t>Invalid E-Mail Address Text</t>
+  </si>
+  <si>
+    <t>Please enter a valid e-mail address.</t>
+  </si>
+  <si>
+    <t>Please check your E-mail inbox for instructions to access your account.</t>
+  </si>
+  <si>
+    <t>Password Sent Header Text</t>
   </si>
 </sst>
 </file>
@@ -631,7 +662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -660,4 +691,58 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified incorrect password expected text
</commit_message>
<xml_diff>
--- a/Login.xlsx
+++ b/Login.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Site URL</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Password Sent Header Text</t>
+  </si>
+  <si>
+    <t>Incorrect user ID or password.</t>
   </si>
 </sst>
 </file>
@@ -599,11 +602,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -619,7 +623,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -697,7 +701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Check forgot password e-mail
</commit_message>
<xml_diff>
--- a/Login.xlsx
+++ b/Login.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>Site URL</t>
   </si>
@@ -124,6 +124,18 @@
   </si>
   <si>
     <t>Incorrect user ID or password.</t>
+  </si>
+  <si>
+    <t>Forgot Password E-Mail Body Text</t>
+  </si>
+  <si>
+    <t>XXX</t>
+  </si>
+  <si>
+    <t>Forgot Password E-Mail Subject Text</t>
+  </si>
+  <si>
+    <t>MicroEdge - Automated</t>
   </si>
 </sst>
 </file>
@@ -602,7 +614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -699,9 +711,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -710,9 +724,11 @@
     <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="64.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -728,8 +744,14 @@
       <c r="E1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -744,6 +766,12 @@
       </c>
       <c r="E2" t="s">
         <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pushing latest, no major changes yet
</commit_message>
<xml_diff>
--- a/Login.xlsx
+++ b/Login.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration" sheetId="2" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="IncorrectUserID" sheetId="5" r:id="rId5"/>
     <sheet name="LoginHeaderFooter" sheetId="6" r:id="rId6"/>
     <sheet name="ForgotPasswordHeaderFooter" sheetId="7" r:id="rId7"/>
+    <sheet name="ForgotPasswordEmail" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>Site URL</t>
   </si>
@@ -68,9 +69,6 @@
   </si>
   <si>
     <t>At vidit veritus duo, erat putent eu qui. Vim an numquam accumsan deserunt. Soluta delectus vim cu, ad nam agam epicuri democritum, ei torquatos scriptorem eum. Putent iracundia intellegat has an, mollis accusata scripserit pri ut. Exerci voluptua disputa</t>
-  </si>
-  <si>
-    <t>Header Text</t>
   </si>
   <si>
     <t>Footer Text</t>
@@ -90,6 +88,57 @@
   </si>
   <si>
     <t>Header Text 2</t>
+  </si>
+  <si>
+    <t>E-Mail Address</t>
+  </si>
+  <si>
+    <t>me.automaton@gmail.com</t>
+  </si>
+  <si>
+    <t>Default E-Mail Address Text</t>
+  </si>
+  <si>
+    <t>Enter e-mail address</t>
+  </si>
+  <si>
+    <t>Missing E-Mail Address Text</t>
+  </si>
+  <si>
+    <t>E-mail Address is Required.</t>
+  </si>
+  <si>
+    <t>Invalid E-Mail Address Text</t>
+  </si>
+  <si>
+    <t>Please enter a valid e-mail address.</t>
+  </si>
+  <si>
+    <t>Please check your E-mail inbox for instructions to access your account.</t>
+  </si>
+  <si>
+    <t>Password Sent Header Text</t>
+  </si>
+  <si>
+    <t>Incorrect user ID or password.</t>
+  </si>
+  <si>
+    <t>Forgot Password E-Mail Body Text</t>
+  </si>
+  <si>
+    <t>XXX</t>
+  </si>
+  <si>
+    <t>Forgot Password E-Mail Subject Text</t>
+  </si>
+  <si>
+    <t>MicroEdge - Automated</t>
+  </si>
+  <si>
+    <t>Footer</t>
+  </si>
+  <si>
+    <t>Header</t>
   </si>
 </sst>
 </file>
@@ -469,7 +518,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -495,7 +546,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -542,7 +595,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -568,11 +623,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -588,7 +646,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -600,30 +658,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="345" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -631,30 +692,100 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some updates: created Android.xml file for android specific testng config. Also add Android option as one of the browsers in the Browser class. Migrated existing login tests into android test.
</commit_message>
<xml_diff>
--- a/Login.xlsx
+++ b/Login.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17040" windowHeight="6810" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,8 @@
     <sheet name="ForgotPasswordHeaderFooter" sheetId="7" r:id="rId7"/>
     <sheet name="ForgotPasswordEmail" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:K20"/>
 </workbook>
 </file>
 
@@ -145,10 +146,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -171,17 +180,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -189,6 +201,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -237,7 +252,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -272,7 +287,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -518,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,11 +548,14 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" location="/page/login"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -658,7 +676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Updated copyright date to 2015
</commit_message>
<xml_diff>
--- a/Login.xlsx
+++ b/Login.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17040" windowHeight="6810" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17040" windowHeight="6810" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,6 @@
     <sheet name="ForgotPasswordEmail" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K20"/>
 </workbook>
 </file>
 
@@ -75,71 +74,71 @@
     <t>Footer Text</t>
   </si>
   <si>
-    <t>© 2014 - Reviewer Connect
+    <t>Please enter your e-mail address in the space provided and click Send.</t>
+  </si>
+  <si>
+    <t>Header Text 1</t>
+  </si>
+  <si>
+    <t>You will receive an e-mail with information for accessing your account.</t>
+  </si>
+  <si>
+    <t>Header Text 2</t>
+  </si>
+  <si>
+    <t>E-Mail Address</t>
+  </si>
+  <si>
+    <t>me.automaton@gmail.com</t>
+  </si>
+  <si>
+    <t>Default E-Mail Address Text</t>
+  </si>
+  <si>
+    <t>Enter e-mail address</t>
+  </si>
+  <si>
+    <t>Missing E-Mail Address Text</t>
+  </si>
+  <si>
+    <t>E-mail Address is Required.</t>
+  </si>
+  <si>
+    <t>Invalid E-Mail Address Text</t>
+  </si>
+  <si>
+    <t>Please enter a valid e-mail address.</t>
+  </si>
+  <si>
+    <t>Please check your E-mail inbox for instructions to access your account.</t>
+  </si>
+  <si>
+    <t>Password Sent Header Text</t>
+  </si>
+  <si>
+    <t>Incorrect user ID or password.</t>
+  </si>
+  <si>
+    <t>Forgot Password E-Mail Body Text</t>
+  </si>
+  <si>
+    <t>XXX</t>
+  </si>
+  <si>
+    <t>Forgot Password E-Mail Subject Text</t>
+  </si>
+  <si>
+    <t>MicroEdge - Automated</t>
+  </si>
+  <si>
+    <t>Footer</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>© 2015 - Reviewer Connect
 Reviewer Connect Description</t>
-  </si>
-  <si>
-    <t>Please enter your e-mail address in the space provided and click Send.</t>
-  </si>
-  <si>
-    <t>Header Text 1</t>
-  </si>
-  <si>
-    <t>You will receive an e-mail with information for accessing your account.</t>
-  </si>
-  <si>
-    <t>Header Text 2</t>
-  </si>
-  <si>
-    <t>E-Mail Address</t>
-  </si>
-  <si>
-    <t>me.automaton@gmail.com</t>
-  </si>
-  <si>
-    <t>Default E-Mail Address Text</t>
-  </si>
-  <si>
-    <t>Enter e-mail address</t>
-  </si>
-  <si>
-    <t>Missing E-Mail Address Text</t>
-  </si>
-  <si>
-    <t>E-mail Address is Required.</t>
-  </si>
-  <si>
-    <t>Invalid E-Mail Address Text</t>
-  </si>
-  <si>
-    <t>Please enter a valid e-mail address.</t>
-  </si>
-  <si>
-    <t>Please check your E-mail inbox for instructions to access your account.</t>
-  </si>
-  <si>
-    <t>Password Sent Header Text</t>
-  </si>
-  <si>
-    <t>Incorrect user ID or password.</t>
-  </si>
-  <si>
-    <t>Forgot Password E-Mail Body Text</t>
-  </si>
-  <si>
-    <t>XXX</t>
-  </si>
-  <si>
-    <t>Forgot Password E-Mail Subject Text</t>
-  </si>
-  <si>
-    <t>MicroEdge - Automated</t>
-  </si>
-  <si>
-    <t>Footer</t>
-  </si>
-  <si>
-    <t>Header</t>
   </si>
 </sst>
 </file>
@@ -252,7 +251,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -287,7 +286,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -533,7 +532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -664,7 +663,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -686,10 +685,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="345" x14ac:dyDescent="0.25">
@@ -697,7 +696,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -710,16 +709,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
         <v>16</v>
@@ -727,13 +726,13 @@
     </row>
     <row r="2" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -762,48 +761,48 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" t="s">
-        <v>30</v>
-      </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>